<commit_message>
Added two quadrant ATAN form
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0444567-C89A-4B81-BCD3-87E168559451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6147319-E01C-419E-91A6-F77A65AB81A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>FROM:</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>_Z</t>
+  </si>
+  <si>
+    <t>https://www.siranah.de/html/sail042e.htm</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +290,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -331,7 +340,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -341,6 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -800,6 +810,50 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>326823</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>503</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7528ADD8-582F-3B1A-9AE9-032478281DBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9753600" y="1200150"/>
+          <a:ext cx="7649643" cy="3600953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1095,7 +1149,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1387,37 +1441,39 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="C7:M12"/>
+  <dimension ref="C2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7">
-        <v>-20</v>
-      </c>
-      <c r="E7">
         <v>49</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="9">
         <v>49</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="9">
         <v>49</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="9">
         <v>49</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="9">
         <v>68</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="9">
         <v>-20</v>
       </c>
     </row>
@@ -1426,27 +1482,23 @@
         <v>22</v>
       </c>
       <c r="D8">
-        <v>22.05</v>
-      </c>
-      <c r="E8">
-        <f>45+11/60</f>
+        <v>12.1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>12.1</v>
+      </c>
+      <c r="J8" s="9">
         <v>45.18333333333333</v>
       </c>
-      <c r="I8">
-        <v>12.1</v>
-      </c>
-      <c r="J8">
-        <v>45.18333333333333</v>
-      </c>
-      <c r="K8">
+      <c r="K8" s="9">
         <f>74+16/60</f>
         <v>74.266666666666666</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="9">
         <f>21+8/60</f>
         <v>21.133333333333333</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="9">
         <f>22+3/60</f>
         <v>22.05</v>
       </c>
@@ -1456,24 +1508,21 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>63</v>
-      </c>
-      <c r="E9">
+        <v>58</v>
+      </c>
+      <c r="I9" s="9">
+        <v>58</v>
+      </c>
+      <c r="J9" s="9">
         <v>259</v>
       </c>
-      <c r="I9">
-        <v>58</v>
-      </c>
-      <c r="J9">
-        <v>259</v>
-      </c>
-      <c r="K9">
+      <c r="K9" s="9">
         <v>347</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="9">
         <v>329</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="9">
         <v>63</v>
       </c>
     </row>
@@ -1487,7 +1536,7 @@
 _xlpm.t,_t*PI()/180,
 _xlpm.d,_d*PI()/180,
 ASIN(COS(_xlpm.L)*COS(_xlpm.d)*COS(_xlpm.t)+SIN(_xlpm.L)*SIN(_xlpm.d))*180/PI())</f>
-        <v>15.486303643338168</v>
+        <v>29.87672961514842</v>
       </c>
       <c r="I11">
         <v>29.87672961514842</v>
@@ -1512,7 +1561,7 @@
 _xlpm.t,_t*PI()/180,
 _xlpm.h,_h*PI()/180,
 ASIN(COS(_xlpm.d)*SIN(_xlpm.t)/COS(_xlpm.h))*180/PI())</f>
-        <v>58.975538982785935</v>
+        <v>72.999137827422672</v>
       </c>
       <c r="I12">
         <v>72.999137827422672</v>
@@ -1525,6 +1574,22 @@
       </c>
       <c r="L12">
         <v>-38.394152431161189</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>_xlfn.LET(
+_xlpm.t,_t*PI()/180,
+_xlpm.L,_L*PI()/180,
+_xlpm.d,_d*PI()/180,
+180/PI()*ATAN2(-SIN(_xlpm.t),COS(_xlpm.L)*TAN(_xlpm.d)-SIN(_xlpm.L)*COS(_xlpm.t)))</f>
+        <v>-162.99913782742269</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>C14+270</f>
+        <v>107.00086217257731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added comment on work needed
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6147319-E01C-419E-91A6-F77A65AB81A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658CC027-883F-4CD0-AB08-7061B6FD1425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>FROM:</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>https://www.siranah.de/html/sail042e.htm</t>
+  </si>
+  <si>
+    <t>I need to understand the definition of azimuth better.</t>
   </si>
 </sst>
 </file>
@@ -673,7 +676,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1" y="0"/>
-          <a:ext cx="2200272" cy="484632"/>
+          <a:ext cx="2198367" cy="492252"/>
           <a:chOff x="3162303" y="274265"/>
           <a:chExt cx="2198368" cy="489383"/>
         </a:xfrm>
@@ -1149,7 +1152,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1441,10 +1444,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="C2:M16"/>
+  <dimension ref="C2:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1590,6 +1593,11 @@
       <c r="C16">
         <f>C14+270</f>
         <v>107.00086217257731</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to get azimuth correct
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658CC027-883F-4CD0-AB08-7061B6FD1425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457B4EA2-60B9-4F37-A0B6-91B910DC5E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,21 @@
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_Alt">Report!$D$23</definedName>
     <definedName name="_d">Report!$D$8</definedName>
     <definedName name="_h">Report!$D$11</definedName>
     <definedName name="_L">Report!$D$7</definedName>
+    <definedName name="_PX">Report!$D$20</definedName>
+    <definedName name="_PZ">Report!$D$21</definedName>
     <definedName name="_t">Report!$D$9</definedName>
     <definedName name="_Z">Report!$D$12</definedName>
+    <definedName name="_ZPA">Report!$D$24</definedName>
+    <definedName name="_ZX">Report!$D$22</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -69,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>FROM:</t>
   </si>
@@ -153,6 +158,24 @@
   </si>
   <si>
     <t>I need to understand the definition of azimuth better.</t>
+  </si>
+  <si>
+    <t>_PX</t>
+  </si>
+  <si>
+    <t>_PZ</t>
+  </si>
+  <si>
+    <t>_ZX</t>
+  </si>
+  <si>
+    <t>_Alt</t>
+  </si>
+  <si>
+    <t>_ZPA</t>
+  </si>
+  <si>
+    <t>https://astronavigationdemystified.com/calculating-azimuth-and-altitude-at-the-assumed-position-by-spherical-trigonometry/</t>
   </si>
 </sst>
 </file>
@@ -676,7 +699,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1" y="0"/>
-          <a:ext cx="2198367" cy="492252"/>
+          <a:ext cx="2200272" cy="484632"/>
           <a:chOff x="3162303" y="274265"/>
           <a:chExt cx="2198368" cy="489383"/>
         </a:xfrm>
@@ -932,8 +955,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3158491" y="270455"/>
-          <a:ext cx="2205990" cy="464875"/>
+          <a:off x="3166111" y="262835"/>
+          <a:ext cx="2200275" cy="455350"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="459814"/>
         </a:xfrm>
@@ -1152,7 +1175,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1444,25 +1467,30 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="C2:M18"/>
+  <dimension ref="C2:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7">
-        <v>49</v>
+        <v>-20</v>
       </c>
       <c r="I7" s="9">
         <v>49</v>
@@ -1479,13 +1507,16 @@
       <c r="M7" s="9">
         <v>-20</v>
       </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8">
-        <v>12.1</v>
+        <v>22.05</v>
       </c>
       <c r="I8" s="9">
         <v>12.1</v>
@@ -1505,13 +1536,16 @@
         <f>22+3/60</f>
         <v>22.05</v>
       </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>28.091666666666665</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I9" s="9">
         <v>58</v>
@@ -1528,8 +1562,11 @@
       <c r="M9" s="9">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>24</v>
       </c>
@@ -1539,7 +1576,11 @@
 _xlpm.t,_t*PI()/180,
 _xlpm.d,_d*PI()/180,
 ASIN(COS(_xlpm.L)*COS(_xlpm.d)*COS(_xlpm.t)+SIN(_xlpm.L)*SIN(_xlpm.d))*180/PI())</f>
-        <v>29.87672961514842</v>
+        <v>15.486303643338168</v>
+      </c>
+      <c r="E11" t="str">
+        <f>INT(_h)&amp;"° "&amp;TEXT(ROUND(MOD(_h,1)*60,1),"0.0")</f>
+        <v>15° 29.2</v>
       </c>
       <c r="I11">
         <v>29.87672961514842</v>
@@ -1553,8 +1594,12 @@
       <c r="L11">
         <v>39.330371718485488</v>
       </c>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <f>32+58/60</f>
+        <v>32.966666666666669</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>25</v>
       </c>
@@ -1564,7 +1609,7 @@
 _xlpm.t,_t*PI()/180,
 _xlpm.h,_h*PI()/180,
 ASIN(COS(_xlpm.d)*SIN(_xlpm.t)/COS(_xlpm.h))*180/PI())</f>
-        <v>72.999137827422672</v>
+        <v>58.975538982785935</v>
       </c>
       <c r="I12">
         <v>72.999137827422672</v>
@@ -1578,26 +1623,100 @@
       <c r="L12">
         <v>-38.394152431161189</v>
       </c>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>_xlfn.LET(
 _xlpm.t,_t*PI()/180,
 _xlpm.L,_L*PI()/180,
 _xlpm.d,_d*PI()/180,
 180/PI()*ATAN2(-SIN(_xlpm.t),COS(_xlpm.L)*TAN(_xlpm.d)-SIN(_xlpm.L)*COS(_xlpm.t)))</f>
-        <v>-162.99913782742269</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <f>C14+270</f>
-        <v>107.00086217257731</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+        <v>148.97553898278593</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>180+C14</f>
+        <v>328.97553898278591</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <f>90-_d</f>
+        <v>67.95</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <f>90-_L</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <f>90-_h</f>
+        <v>74.513696356661825</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <f>90-_ZX</f>
+        <v>15.486303643338175</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <f>_t</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f>(COS(_PX*PI()/180)-COS(_ZX*PI()/180)*COS(_PZ*PI()/180))/(SIN(_ZX*PI()/180)*SIN(_PZ*PI()/180))</f>
+        <v>0.51540397435955743</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f>ACOS(C26)*180/PI()</f>
+        <v>58.975538982785935</v>
+      </c>
+      <c r="D27" t="str">
+        <f>INT(C27)&amp;"° "&amp;TEXT(ROUND(MOD(C27,1)*60,1),"0.0")</f>
+        <v>58° 58.5</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>180-C27</f>
+        <v>121.02446101721407</v>
+      </c>
+      <c r="D28" t="str">
+        <f>INT(C28)&amp;"° "&amp;TEXT(ROUND(MOD(C28,1)*60,1),"0.0")</f>
+        <v>121° 1.5</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1764,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>22-May-2025</v>
+        <v>23-May-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1941,7 +2060,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>22-May-2025</v>
+        <v>23-May-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Getting close to understanding the navigation triangle
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772FD381-A988-494C-9B81-427C1FB54056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AB7766-19B4-48A5-8172-FDDC9892F822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21160" yWindow="0" windowWidth="21230" windowHeight="19590" firstSheet="1" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula208" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="4" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
   <si>
     <t>FROM:</t>
   </si>
@@ -841,7 +841,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1" y="0"/>
-          <a:ext cx="2201542" cy="479552"/>
+          <a:ext cx="2200272" cy="484632"/>
           <a:chOff x="3162303" y="274265"/>
           <a:chExt cx="2198368" cy="489383"/>
         </a:xfrm>
@@ -1508,8 +1508,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3171191" y="257755"/>
-          <a:ext cx="2196465" cy="449000"/>
+          <a:off x="3166111" y="262835"/>
+          <a:ext cx="2200275" cy="455350"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="459814"/>
         </a:xfrm>
@@ -1728,7 +1728,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -2038,6 +2038,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -2327,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E99B084-70EE-4F78-B076-1D78244F5ECF}">
   <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2881,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6FCC6-3E31-4FC6-8F07-E8D73C1C42B1}">
   <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3067,14 +3070,14 @@
       <c r="I9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>62</v>
+      <c r="J9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -3090,15 +3093,13 @@
       <c r="I10" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>63</v>
-      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -3111,9 +3112,6 @@
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11">_fHM(C11)</f>
         <v>37° 38.6'</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First time I think I understand the algorithm
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0F32F7-4391-40E3-A434-D9E0CBAFA676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC439DD1-933D-479F-9898-CE815EF9D47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-20565" yWindow="1485" windowWidth="23235" windowHeight="11235" firstSheet="2" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula208" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -851,7 +851,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1" y="0"/>
-          <a:ext cx="2200272" cy="484632"/>
+          <a:ext cx="2198367" cy="492252"/>
           <a:chOff x="3162303" y="274265"/>
           <a:chExt cx="2198368" cy="489383"/>
         </a:xfrm>
@@ -1357,16 +1357,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>500380</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>387985</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>217437</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>95851</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>93612</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>72991</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1389,8 +1389,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="500380" y="6122670"/>
-          <a:ext cx="11009897" cy="4366861"/>
+          <a:off x="1607185" y="5730240"/>
+          <a:ext cx="10990847" cy="4458301"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1454,7 +1454,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>3289</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>71236</xdr:rowOff>
+      <xdr:rowOff>55996</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1562,8 +1562,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3166111" y="262835"/>
-          <a:ext cx="2200275" cy="455350"/>
+          <a:off x="3158491" y="270455"/>
+          <a:ext cx="2205990" cy="464875"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="459814"/>
         </a:xfrm>
@@ -1782,7 +1782,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -2071,7 +2071,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="841" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="662" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="974" row="9">
@@ -2938,10 +2938,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6FCC6-3E31-4FC6-8F07-E8D73C1C42B1}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3005,7 +3005,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="13">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="F5">
         <v>15</v>
@@ -3034,7 +3034,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="13">
-        <v>-26.378333333333334</v>
+        <v>21.156666666666666</v>
       </c>
       <c r="F6">
         <v>19.315000000000001</v>
@@ -3066,7 +3066,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="13">
-        <v>33</v>
+        <v>284</v>
       </c>
       <c r="F7">
         <v>65</v>
@@ -3163,24 +3163,44 @@
       </c>
       <c r="C11">
         <f>_xlfn.LET(_xlpm.L, PI() / 180 * _L, _xlpm.d, PI() / 180 * _d, _xlpm.t, PI() / 180 * _t, ASIN(SIN(_xlpm.L) * SIN(_xlpm.d) + COS(_xlpm.L) * COS(_xlpm.d) * COS(_xlpm.t)) * 180 / PI())</f>
-        <v>37.644050023822807</v>
+        <v>12.666886583405681</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11">_fHM(C11)</f>
-        <v>37° 38.6'</v>
+        <v>12° 40.0'</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12">
-        <f>_xlfn.LET(_xlpm.d, PI() / 180 * _d, _xlpm.L, PI() / 180 * _L, _xlpm.t, PI() / 180 * _t, _xlpm.s, SIN(_xlpm.d), _xlpm.c, COS(_xlpm.d) * COS(_xlpm.t), _xlpm.res, ASIN(SIN(_xlpm.L) * SIN(_xlpm.d) + COS(_xlpm.L) * COS(_xlpm.d) * COS(_xlpm.t)), _xlpm.x, DEGREES(ACOS((_xlpm.s * COS(_xlpm.L) - _xlpm.c * SIN(_xlpm.L)) / COS(_xlpm.res))), _xlpm.a, IF(SIGN(_xlpm.d) &lt;&gt; SIGN(_xlpm.L), 180 - _xlpm.x, _xlpm.x), _xlpm.a)</f>
-        <v>38.0402181944944</v>
+      <c r="C12" cm="1">
+        <f t="array" ref="C12">_xlfn.LAMBDA(_xlpm.dec,_xlpm.Lat,_xlpm.LHA,
+_xlfn.LET(_xlpm.f, IF(SIGN(_xlpm.dec)&lt;&gt;SIGN(_xlpm.Lat),-1,1),
+    _xlpm.d, PI() / 180 * ABS(_xlpm.dec),
+    _xlpm.L, PI() / 180 * ABS(_xlpm.Lat) * _xlpm.f,
+    _xlpm.t, PI() / 180 * _xlpm.LHA,
+    _xlpm.s, SIN(_xlpm.d),
+    _xlpm.c, COS(_xlpm.d) * COS(_xlpm.t),
+    _xlpm.res, ASIN(SIN(_xlpm.L) * SIN(_xlpm.d) + COS(_xlpm.L) * COS(_xlpm.d) * COS(_xlpm.t)),
+    _xlpm.x, DEGREES(ACOS((_xlpm.s * COS(_xlpm.L) - _xlpm.c * SIN(_xlpm.L)) / COS(_xlpm.res))),
+    IF(_xlpm.f=-1,180-_xlpm.x,_xlpm.x)
+))(_d,_L,_t)</f>
+        <v>111.95647513034474</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" ref="D12">_fHM(ABS(C12))</f>
-        <v>38° 2.4'</v>
+        <v>111° 57.4'</v>
+      </c>
+      <c r="K12">
+        <f>(L6-21)*60</f>
+        <v>9.3999999999999773</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>21+9.4/60</f>
+        <v>21.156666666666666</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -3239,7 +3259,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>24-May-2025</v>
+        <v>26-May-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3535,7 +3555,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>24-May-2025</v>
+        <v>26-May-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added v and d correction example
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC439DD1-933D-479F-9898-CE815EF9D47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA67C46-FD27-4620-B9CD-B3969131893B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20565" yWindow="1485" windowWidth="23235" windowHeight="11235" firstSheet="2" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-25410" yWindow="0" windowWidth="23235" windowHeight="15585" firstSheet="2" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula208" sheetId="1" r:id="rId1"/>
     <sheet name="Formula229" sheetId="4" r:id="rId2"/>
     <sheet name="Formula229 (2)" sheetId="6" r:id="rId3"/>
     <sheet name="Formula229 (3)" sheetId="7" r:id="rId4"/>
-    <sheet name="Formats" sheetId="2" r:id="rId5"/>
-    <sheet name="Lists" sheetId="3" r:id="rId6"/>
+    <sheet name="vCorrection" sheetId="8" r:id="rId5"/>
+    <sheet name="Formats" sheetId="2" r:id="rId6"/>
+    <sheet name="Lists" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Alt">Formula208!$D$23</definedName>
@@ -48,7 +49,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
   <si>
     <t>FROM:</t>
   </si>
@@ -1494,6 +1495,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>16943</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>55637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B03231-F7A5-5C6E-77CB-C632E1303B5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="171450"/>
+          <a:ext cx="12203228" cy="2810267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2938,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6FCC6-3E31-4FC6-8F07-E8D73C1C42B1}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G11" sqref="G11"/>
@@ -3222,6 +3272,68 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C74FBC-AF29-42D0-B973-6A56AE2E1348}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str" cm="1">
+        <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
+        <v>26-May-2025</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>19+10/60</f>
+        <v>19.166666666666668</v>
+      </c>
+      <c r="H24">
+        <f>G24/60</f>
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="I24">
+        <f>12.1*H24</f>
+        <v>3.865277777777778</v>
+      </c>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f>H24*-8.9</f>
+        <v>-2.8430555555555559</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -3520,7 +3632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>

</xml_diff>

<commit_message>
Working on a numerical method to solve triangle
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -1,55 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA67C46-FD27-4620-B9CD-B3969131893B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DAAA49-0B6F-420D-9566-23466086243E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25410" yWindow="0" windowWidth="23235" windowHeight="15585" firstSheet="2" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula208" sheetId="1" r:id="rId1"/>
     <sheet name="Formula229" sheetId="4" r:id="rId2"/>
     <sheet name="Formula229 (2)" sheetId="6" r:id="rId3"/>
-    <sheet name="Formula229 (3)" sheetId="7" r:id="rId4"/>
-    <sheet name="vCorrection" sheetId="8" r:id="rId5"/>
-    <sheet name="Formats" sheetId="2" r:id="rId6"/>
-    <sheet name="Lists" sheetId="3" r:id="rId7"/>
+    <sheet name="Working" sheetId="7" r:id="rId4"/>
+    <sheet name="NumMethod" sheetId="9" r:id="rId5"/>
+    <sheet name="vCorrection" sheetId="8" r:id="rId6"/>
+    <sheet name="Formats" sheetId="2" r:id="rId7"/>
+    <sheet name="Lists" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_Alt">Formula208!$D$23</definedName>
     <definedName name="_d" localSheetId="1">Formula229!$C$6</definedName>
     <definedName name="_d" localSheetId="2">'Formula229 (2)'!$C$6</definedName>
-    <definedName name="_d" localSheetId="3">'Formula229 (3)'!$C$6</definedName>
+    <definedName name="_d" localSheetId="4">NumMethod!$C$6</definedName>
+    <definedName name="_d" localSheetId="3">Working!$C$6</definedName>
     <definedName name="_d">Formula208!$D$8</definedName>
     <definedName name="_fHM">_xlfn.LAMBDA(_xlpm.a, INT(_xlpm.a) &amp; "° " &amp; FIXED(MOD(_xlpm.a, 1) * 60, 1) &amp; "'")</definedName>
     <definedName name="_h">Formula208!$D$11</definedName>
     <definedName name="_HC" comment="Computed altitude_x000a_" localSheetId="1">Formula229!$D$11</definedName>
     <definedName name="_HC" comment="Computed altitude_x000a_" localSheetId="2">'Formula229 (2)'!$D$11</definedName>
-    <definedName name="_HC" comment="Computed altitude_x000a_" localSheetId="3">'Formula229 (3)'!$D$11</definedName>
+    <definedName name="_HC" comment="Computed altitude_x000a_" localSheetId="4">NumMethod!$D$11</definedName>
+    <definedName name="_HC" comment="Computed altitude_x000a_" localSheetId="3">Working!$D$11</definedName>
     <definedName name="_L" localSheetId="1">Formula229!$C$5</definedName>
     <definedName name="_L" localSheetId="2">'Formula229 (2)'!$C$5</definedName>
-    <definedName name="_L" localSheetId="3">'Formula229 (3)'!$C$5</definedName>
+    <definedName name="_L" localSheetId="4">NumMethod!$C$5</definedName>
+    <definedName name="_L" localSheetId="3">Working!$C$5</definedName>
     <definedName name="_L">Formula208!$D$7</definedName>
     <definedName name="_PX">Formula208!$D$20</definedName>
     <definedName name="_PZ">Formula208!$D$21</definedName>
     <definedName name="_t" localSheetId="1">Formula229!$C$7</definedName>
     <definedName name="_t" localSheetId="2">'Formula229 (2)'!$C$7</definedName>
-    <definedName name="_t" localSheetId="3">'Formula229 (3)'!$C$7</definedName>
+    <definedName name="_t" localSheetId="4">NumMethod!$C$7</definedName>
+    <definedName name="_t" localSheetId="3">Working!$C$7</definedName>
     <definedName name="_t">Formula208!$D$9</definedName>
     <definedName name="_Z">Formula208!$D$12</definedName>
     <definedName name="_ZPA">Formula208!$D$24</definedName>
     <definedName name="_ZX">Formula208!$D$22</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">NumMethod!$C$7</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">NumMethod!$C$11</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">12.66688658</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -91,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="73">
   <si>
     <t>FROM:</t>
   </si>
@@ -295,6 +327,21 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>LHA</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>Body Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured </t>
   </si>
 </sst>
 </file>
@@ -852,7 +899,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1" y="0"/>
-          <a:ext cx="2198367" cy="492252"/>
+          <a:ext cx="2200272" cy="484632"/>
           <a:chOff x="3162303" y="274265"/>
           <a:chExt cx="2198368" cy="489383"/>
         </a:xfrm>
@@ -1495,6 +1542,187 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>34554</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{110D2269-2A1D-4FA7-B3BB-3BAEE0F3A4BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11292840" y="335280"/>
+          <a:ext cx="11007354" cy="3635240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>387985</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>360312</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>72991</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E179798C-7800-46F6-A07C-D020C1713803}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607185" y="5604510"/>
+          <a:ext cx="10998467" cy="4359241"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>569369</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>110642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A50AEEE8-8A74-4BE5-881A-7E8A875345EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4998720" y="2514600"/>
+          <a:ext cx="7473089" cy="1116482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>269989</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>55996</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60BC7C89-CD98-427E-91D1-A0E554C4472C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2598420" y="8938260"/>
+          <a:ext cx="9916909" cy="5367136"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1540,7 +1768,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1612,8 +1840,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3158491" y="270455"/>
-          <a:ext cx="2205990" cy="464875"/>
+          <a:off x="3166111" y="262835"/>
+          <a:ext cx="2200275" cy="455350"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="459814"/>
         </a:xfrm>
@@ -2697,8 +2925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916FFC01-0787-4116-93FD-519DFE4BC403}">
   <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2988,10 +3216,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6FCC6-3E31-4FC6-8F07-E8D73C1C42B1}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3057,6 +3285,9 @@
       <c r="C5" s="13">
         <v>-1</v>
       </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
       <c r="F5">
         <v>15</v>
       </c>
@@ -3086,6 +3317,9 @@
       <c r="C6" s="13">
         <v>21.156666666666666</v>
       </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
       <c r="F6">
         <v>19.315000000000001</v>
       </c>
@@ -3117,6 +3351,9 @@
       </c>
       <c r="C7" s="13">
         <v>284</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
       </c>
       <c r="F7">
         <v>65</v>
@@ -3272,10 +3509,310 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14A46DE-C8B5-46AB-B5C3-3D9A24AAEFAD}">
+  <dimension ref="B2:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="D11" sqref="D11:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>49</v>
+      </c>
+      <c r="J5">
+        <v>49</v>
+      </c>
+      <c r="K5">
+        <v>49</v>
+      </c>
+      <c r="L5" s="14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="13">
+        <v>21.156666666666666</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6">
+        <v>19.315000000000001</v>
+      </c>
+      <c r="G6">
+        <v>-26.378333333333334</v>
+      </c>
+      <c r="H6">
+        <v>12.581666666666667</v>
+      </c>
+      <c r="I6">
+        <f>12+6/60</f>
+        <v>12.1</v>
+      </c>
+      <c r="J6">
+        <f>45+11/60</f>
+        <v>45.18333333333333</v>
+      </c>
+      <c r="K6">
+        <f>74+16/60</f>
+        <v>74.266666666666666</v>
+      </c>
+      <c r="L6" s="14">
+        <v>21.156666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="13">
+        <v>284.00000049884716</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>58</v>
+      </c>
+      <c r="J7">
+        <v>259</v>
+      </c>
+      <c r="K7">
+        <v>347</v>
+      </c>
+      <c r="L7" s="14">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <f>_xlfn.LET(_xlpm.L, PI() / 180 * _L, _xlpm.d, PI() / 180 * _d, _xlpm.t, PI() / 180 * _t, ASIN(SIN(_xlpm.L) * SIN(_xlpm.d) + COS(_xlpm.L) * COS(_xlpm.d) * COS(_xlpm.t)) * 180 / PI())</f>
+        <v>12.666887046000065</v>
+      </c>
+      <c r="D11" t="str" cm="1">
+        <f t="array" ref="D11">_fHM(C11)</f>
+        <v>12° 40.0'</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="9">
+        <v>12.666886597987773</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" cm="1">
+        <f t="array" ref="C12">_xlfn.LAMBDA(_xlpm.dec,_xlpm.Lat,_xlpm.LHA,
+_xlfn.LET(_xlpm.f, IF(SIGN(_xlpm.dec)&lt;&gt;SIGN(_xlpm.Lat),-1,1),
+    _xlpm.d, PI() / 180 * ABS(_xlpm.dec),
+    _xlpm.L, PI() / 180 * ABS(_xlpm.Lat) * _xlpm.f,
+    _xlpm.t, PI() / 180 * _xlpm.LHA,
+    _xlpm.s, SIN(_xlpm.d),
+    _xlpm.c, COS(_xlpm.d) * COS(_xlpm.t),
+    _xlpm.res, ASIN(SIN(_xlpm.L) * SIN(_xlpm.d) + COS(_xlpm.L) * COS(_xlpm.d) * COS(_xlpm.t)),
+    _xlpm.x, DEGREES(ACOS((_xlpm.s * COS(_xlpm.L) - _xlpm.c * SIN(_xlpm.L)) / COS(_xlpm.res))),
+    IF(_xlpm.f=-1,180-_xlpm.x,_xlpm.x)
+))(_d,_L,_t)</f>
+        <v>111.95647518096528</v>
+      </c>
+      <c r="D12" t="str" cm="1">
+        <f t="array" ref="D12">_fHM(ABS(C12))</f>
+        <v>111° 57.4'</v>
+      </c>
+      <c r="K12">
+        <f>(L6-21)*60</f>
+        <v>9.3999999999999773</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>21+9.4/60</f>
+        <v>21.156666666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C74FBC-AF29-42D0-B973-6A56AE2E1348}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -3303,7 +3840,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>26-May-2025</v>
+        <v>04-Jun-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3333,7 +3870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -3371,7 +3908,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>26-May-2025</v>
+        <v>04-Jun-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3632,7 +4169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -3667,7 +4204,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>26-May-2025</v>
+        <v>04-Jun-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
My numerical thoughts are good. It seems that I need to have at least two and preferably three celestial objects that I can solve simulataneously.
</commit_message>
<xml_diff>
--- a/SphericalTrig4Nav.xlsx
+++ b/SphericalTrig4Nav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DAAA49-0B6F-420D-9566-23466086243E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3811723E-D3C1-4EBC-9C18-6A4E93AACA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -338,17 +338,17 @@
     <t>dec</t>
   </si>
   <si>
-    <t>Body Data</t>
-  </si>
-  <si>
     <t xml:space="preserve">Measured </t>
+  </si>
+  <si>
+    <t>Celestial Body Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -443,6 +443,14 @@
       <sz val="10"/>
       <name val="Consolas"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -557,7 +565,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -577,6 +585,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -1716,6 +1725,102 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77BCA63D-B396-52C8-DC4C-2924470E3C59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1478280" y="2644140"/>
+          <a:ext cx="4168140" cy="2834640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>I have been so focused on understanding the paper</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> algorithm that I have not looked at the deeply at the problem. The LOP of position approach is simply a graphical approach for solving two nonlinear equations.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Another approach is to use either goal seek or solver to find the LHA value gives the measured altitude of the celestial object. Once you have the LHA value that gives you the measured altitude, you can then compute the azimuth.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>LHA and azimuth allow me to plot my LOP. I need to understand LOP plotting better. It is time for some practice on a chart. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3515,7 +3620,7 @@
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11:D12"/>
+      <selection pane="topRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3555,8 +3660,8 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>71</v>
+      <c r="C4" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="F4" t="s">
         <v>44</v>
@@ -3650,7 +3755,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="13">
-        <v>284.00000049884716</v>
+        <v>283.99999974070147</v>
       </c>
       <c r="D7" t="s">
         <v>69</v>
@@ -3750,14 +3855,14 @@
       </c>
       <c r="C11">
         <f>_xlfn.LET(_xlpm.L, PI() / 180 * _L, _xlpm.d, PI() / 180 * _d, _xlpm.t, PI() / 180 * _t, ASIN(SIN(_xlpm.L) * SIN(_xlpm.d) + COS(_xlpm.L) * COS(_xlpm.d) * COS(_xlpm.t)) * 180 / PI())</f>
-        <v>12.666887046000065</v>
+        <v>12.666886342951196</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11">_fHM(C11)</f>
         <v>12° 40.0'</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="9">
         <v>12.666886597987773</v>
@@ -3779,7 +3884,7 @@
     _xlpm.x, DEGREES(ACOS((_xlpm.s * COS(_xlpm.L) - _xlpm.c * SIN(_xlpm.L)) / COS(_xlpm.res))),
     IF(_xlpm.f=-1,180-_xlpm.x,_xlpm.x)
 ))(_d,_L,_t)</f>
-        <v>111.95647518096528</v>
+        <v>111.95647510403241</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" ref="D12">_fHM(ABS(C12))</f>

</xml_diff>